<commit_message>
Added sheets for 1cm and .5cm intervals
</commit_message>
<xml_diff>
--- a/SensorCalibration.xlsx
+++ b/SensorCalibration.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hope\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yewheng/Desktop/CZ3004-MDP-Arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86B22931-B6EF-4020-BBEA-6D91C5827DA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBC44AF-1364-9145-9DDB-35B55BF910EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2238A5C0-9490-7B40-8416-1163AD9190C2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="2" xr2:uid="{2238A5C0-9490-7B40-8416-1163AD9190C2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="01 Oct (2cm Interval)" sheetId="1" r:id="rId1"/>
+    <sheet name="02 Oct (1cm Interval)" sheetId="2" r:id="rId2"/>
+    <sheet name="02 Oct (0.5cm Interval)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
   <si>
     <t>SRSensorFront1</t>
   </si>
@@ -66,6 +68,15 @@
   </si>
   <si>
     <t>1.0237x10^7</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -114,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,6 +135,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -440,20 +460,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D985BE75-941B-D040-B09A-9504C5CE2441}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3" customWidth="1"/>
     <col min="2" max="7" width="20.83203125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="10.6640625" style="3"/>
+    <col min="8" max="9" width="10.6640625" style="3"/>
+    <col min="10" max="15" width="20.83203125" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="10.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -473,8 +495,27 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I1"/>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -494,8 +535,29 @@
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1">
+        <v>4928.71</v>
+      </c>
+      <c r="K2" s="1">
+        <v>16093.6</v>
+      </c>
+      <c r="L2" s="1">
+        <v>3840.37</v>
+      </c>
+      <c r="M2" s="1">
+        <v>13483.7</v>
+      </c>
+      <c r="N2" s="1">
+        <v>14166.9</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -505,14 +567,29 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="I3" s="3">
-        <v>16</v>
-      </c>
-      <c r="J3" s="3">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1">
+        <v>4.6270899999999999</v>
+      </c>
+      <c r="K3" s="1">
+        <v>14.437099999999999</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2.3652899999999999</v>
+      </c>
+      <c r="M3" s="1">
+        <v>11.9145</v>
+      </c>
+      <c r="N3" s="1">
+        <v>12.313700000000001</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1034.72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -532,14 +609,29 @@
         <v>660</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="I4" s="3">
-        <v>20</v>
-      </c>
-      <c r="J4" s="3">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1">
+        <v>-48.6083</v>
+      </c>
+      <c r="K4" s="1">
+        <v>157.702</v>
+      </c>
+      <c r="L4" s="1">
+        <v>-105.74</v>
+      </c>
+      <c r="M4" s="1">
+        <v>135.04599999999999</v>
+      </c>
+      <c r="N4" s="1">
+        <v>139.66399999999999</v>
+      </c>
+      <c r="O4" s="1">
+        <v>9211.9699999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>6</v>
       </c>
@@ -559,14 +651,8 @@
         <v>677</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="I5" s="3">
-        <v>24</v>
-      </c>
-      <c r="J5" s="3">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>8</v>
       </c>
@@ -586,14 +672,8 @@
         <v>658</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="I6" s="3">
-        <v>28</v>
-      </c>
-      <c r="J6" s="3">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -613,14 +693,8 @@
         <v>504</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="I7" s="3">
-        <v>32</v>
-      </c>
-      <c r="J7" s="3">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>12</v>
       </c>
@@ -640,14 +714,8 @@
         <v>440</v>
       </c>
       <c r="G8" s="2"/>
-      <c r="I8" s="3">
-        <v>36</v>
-      </c>
-      <c r="J8" s="3">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>14</v>
       </c>
@@ -667,14 +735,8 @@
         <v>371</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="I9" s="3">
-        <v>40</v>
-      </c>
-      <c r="J9" s="3">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>16</v>
       </c>
@@ -696,14 +758,8 @@
       <c r="G10" s="1">
         <v>550</v>
       </c>
-      <c r="I10" s="3">
-        <v>44</v>
-      </c>
-      <c r="J10" s="3">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>18</v>
       </c>
@@ -723,14 +779,8 @@
         <v>296</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="I11" s="3">
-        <v>48</v>
-      </c>
-      <c r="J11" s="3">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>20</v>
       </c>
@@ -752,14 +802,8 @@
       <c r="G12" s="1">
         <v>484</v>
       </c>
-      <c r="I12" s="3">
-        <v>52</v>
-      </c>
-      <c r="J12" s="3">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>22</v>
       </c>
@@ -779,14 +823,8 @@
         <v>257</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="I13" s="3">
-        <v>56</v>
-      </c>
-      <c r="J13" s="3">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>24</v>
       </c>
@@ -808,14 +846,8 @@
       <c r="G14" s="1">
         <v>447</v>
       </c>
-      <c r="I14" s="3">
-        <v>60</v>
-      </c>
-      <c r="J14" s="3">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>26</v>
       </c>
@@ -835,14 +867,8 @@
         <v>227</v>
       </c>
       <c r="G15" s="2"/>
-      <c r="I15" s="3">
-        <v>64</v>
-      </c>
-      <c r="J15" s="3">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>28</v>
       </c>
@@ -864,14 +890,8 @@
       <c r="G16" s="1">
         <v>420</v>
       </c>
-      <c r="I16" s="3">
-        <v>68</v>
-      </c>
-      <c r="J16" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>30</v>
       </c>
@@ -891,14 +911,8 @@
         <v>199</v>
       </c>
       <c r="G17" s="2"/>
-      <c r="I17" s="3">
-        <v>72</v>
-      </c>
-      <c r="J17" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>32</v>
       </c>
@@ -920,14 +934,8 @@
       <c r="G18" s="1">
         <v>376</v>
       </c>
-      <c r="I18" s="3">
-        <v>76</v>
-      </c>
-      <c r="J18" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>34</v>
       </c>
@@ -947,14 +955,8 @@
         <v>170</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="I19" s="3">
-        <v>80</v>
-      </c>
-      <c r="J19" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>36</v>
       </c>
@@ -977,7 +979,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>38</v>
       </c>
@@ -998,7 +1000,7 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>40</v>
       </c>
@@ -1021,7 +1023,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42</v>
       </c>
@@ -1032,7 +1034,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44</v>
       </c>
@@ -1045,7 +1047,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>46</v>
       </c>
@@ -1056,7 +1058,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>48</v>
       </c>
@@ -1069,7 +1071,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>50</v>
       </c>
@@ -1080,7 +1082,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>52</v>
       </c>
@@ -1093,7 +1095,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>54</v>
       </c>
@@ -1104,7 +1106,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>56</v>
       </c>
@@ -1117,7 +1119,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>58</v>
       </c>
@@ -1128,7 +1130,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>60</v>
       </c>
@@ -1141,7 +1143,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>62</v>
       </c>
@@ -1152,7 +1154,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>64</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>66</v>
       </c>
@@ -1176,7 +1178,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>68</v>
       </c>
@@ -1189,7 +1191,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>70</v>
       </c>
@@ -1200,7 +1202,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>72</v>
       </c>
@@ -1213,7 +1215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>74</v>
       </c>
@@ -1224,7 +1226,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>76</v>
       </c>
@@ -1237,7 +1239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>78</v>
       </c>
@@ -1248,7 +1250,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>80</v>
       </c>
@@ -1261,7 +1263,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1269,7 +1271,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -1292,7 +1294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>8</v>
       </c>
@@ -1315,7 +1317,7 @@
         <v>1034.72</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>9</v>
       </c>
@@ -1336,6 +1338,1564 @@
       </c>
       <c r="G46" s="3">
         <v>9211.9699999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272BC585-879A-D54C-8DC8-951D497B05AE}">
+  <dimension ref="A1:O52"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="7" width="20.83203125" customWidth="1"/>
+    <col min="10" max="15" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1682CA-3BD7-CA42-8A85-53F8AFB35EE2}">
+  <dimension ref="A1:O102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="7" width="20.83203125" customWidth="1"/>
+    <col min="10" max="15" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="7"/>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>7</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>8</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>10</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>11</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>12</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>13</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>14</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>15</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>16</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>17</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>18</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>18.5</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>19</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>20</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>21</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>22</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>23</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>24</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>25</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code for 02/10 Run
</commit_message>
<xml_diff>
--- a/SensorCalibration.xlsx
+++ b/SensorCalibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yewheng/Desktop/CZ3004-MDP-Arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBC44AF-1364-9145-9DDB-35B55BF910EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8814784C-7A11-2645-A642-027F418F061C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="2" xr2:uid="{2238A5C0-9490-7B40-8416-1163AD9190C2}"/>
+    <workbookView xWindow="16860" yWindow="480" windowWidth="11940" windowHeight="16220" activeTab="1" xr2:uid="{2238A5C0-9490-7B40-8416-1163AD9190C2}"/>
   </bookViews>
   <sheets>
     <sheet name="01 Oct (2cm Interval)" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
   <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.25"/>
@@ -1347,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272BC585-879A-D54C-8DC8-951D497B05AE}">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1536,7 +1536,9 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5">
+        <v>455.6</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1547,8 +1549,12 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="5">
+        <v>422</v>
+      </c>
+      <c r="C12" s="5">
+        <v>517</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1558,8 +1564,12 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="5">
+        <v>394.8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>477</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -1569,8 +1579,12 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="5">
+        <v>364.9</v>
+      </c>
+      <c r="C14" s="5">
+        <v>446</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1580,8 +1594,12 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="5">
+        <v>351.1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>413</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1591,8 +1609,12 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="B16" s="5">
+        <v>328.9</v>
+      </c>
+      <c r="C16" s="5">
+        <v>389</v>
+      </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1602,8 +1624,12 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="B17" s="5">
+        <v>317.5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>367</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1613,8 +1639,12 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="5">
+        <v>300.8</v>
+      </c>
+      <c r="C18" s="5">
+        <v>348</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1624,8 +1654,12 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="B19" s="5">
+        <v>284.5</v>
+      </c>
+      <c r="C19" s="5">
+        <v>329</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1635,8 +1669,12 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="5">
+        <v>277</v>
+      </c>
+      <c r="C20" s="5">
+        <v>314</v>
+      </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1646,8 +1684,12 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="5">
+        <v>265</v>
+      </c>
+      <c r="C21" s="5">
+        <v>300</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1657,8 +1699,12 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="5">
+        <v>256.7</v>
+      </c>
+      <c r="C22" s="5">
+        <v>288</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1668,8 +1714,12 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="5">
+        <v>251.2</v>
+      </c>
+      <c r="C23" s="5">
+        <v>274</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1679,8 +1729,12 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="5">
+        <v>245.3</v>
+      </c>
+      <c r="C24" s="5">
+        <v>259</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1690,8 +1744,12 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="B25" s="5">
+        <v>235</v>
+      </c>
+      <c r="C25" s="5">
+        <v>248</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1701,8 +1759,12 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="B26" s="5">
+        <v>228</v>
+      </c>
+      <c r="C26" s="5">
+        <v>243</v>
+      </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -1712,8 +1774,12 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="5">
+        <v>221</v>
+      </c>
+      <c r="C27" s="5">
+        <v>236</v>
+      </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1723,8 +1789,12 @@
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="B28" s="5">
+        <v>222.9</v>
+      </c>
+      <c r="C28" s="5">
+        <v>226</v>
+      </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1734,8 +1804,12 @@
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="5">
+        <v>213.6</v>
+      </c>
+      <c r="C29" s="5">
+        <v>218</v>
+      </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -1745,8 +1819,12 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="B30" s="5">
+        <v>208.8</v>
+      </c>
+      <c r="C30" s="5">
+        <v>213</v>
+      </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -1756,8 +1834,12 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="B31" s="5">
+        <v>201</v>
+      </c>
+      <c r="C31" s="5">
+        <v>207</v>
+      </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1767,9 +1849,15 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="B32" s="5">
+        <v>196</v>
+      </c>
+      <c r="C32" s="5">
+        <v>204</v>
+      </c>
+      <c r="D32" s="5">
+        <v>203</v>
+      </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -1778,9 +1866,13 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="5">
+        <v>191.6</v>
+      </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="5">
+        <v>193</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -1791,7 +1883,9 @@
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="5">
+        <v>187</v>
+      </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -1802,7 +1896,9 @@
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="5">
+        <v>183</v>
+      </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -1813,7 +1909,9 @@
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="5">
+        <v>180</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -1824,7 +1922,9 @@
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="5">
+        <v>174</v>
+      </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -1835,7 +1935,9 @@
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="D38" s="5">
+        <v>171</v>
+      </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -1846,7 +1948,9 @@
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="D39" s="5">
+        <v>161</v>
+      </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -1857,7 +1961,9 @@
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="D40" s="5">
+        <v>166</v>
+      </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -1868,7 +1974,9 @@
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="D41" s="5">
+        <v>157</v>
+      </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
@@ -1879,7 +1987,9 @@
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="5">
+        <v>158</v>
+      </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
@@ -1890,7 +2000,9 @@
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="5">
+        <v>152</v>
+      </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -1901,7 +2013,9 @@
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="D44" s="5">
+        <v>147</v>
+      </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -1912,7 +2026,9 @@
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+      <c r="D45" s="5">
+        <v>142</v>
+      </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -1923,7 +2039,9 @@
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="D46" s="5">
+        <v>138</v>
+      </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -1934,7 +2052,9 @@
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="D47" s="5">
+        <v>132</v>
+      </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
@@ -1945,7 +2065,9 @@
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+      <c r="D48" s="5">
+        <v>131</v>
+      </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -1956,7 +2078,9 @@
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="D49" s="5">
+        <v>128</v>
+      </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
@@ -1967,7 +2091,9 @@
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="D50" s="5">
+        <v>124</v>
+      </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
@@ -1978,7 +2104,9 @@
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="D51" s="5">
+        <v>137</v>
+      </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
@@ -1989,10 +2117,180 @@
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="D52" s="5">
+        <v>144</v>
+      </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
+    </row>
+    <row r="54" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>30</v>
+      </c>
+      <c r="B54" s="5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>31</v>
+      </c>
+      <c r="B55" s="5">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>32</v>
+      </c>
+      <c r="B56" s="5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>33</v>
+      </c>
+      <c r="B57" s="5">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>34</v>
+      </c>
+      <c r="B58" s="5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>35</v>
+      </c>
+      <c r="B59" s="5">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>36</v>
+      </c>
+      <c r="B60" s="5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>37</v>
+      </c>
+      <c r="B61" s="5">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>38</v>
+      </c>
+      <c r="B62" s="5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>39</v>
+      </c>
+      <c r="B63" s="5">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>40</v>
+      </c>
+      <c r="B64" s="5">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>41</v>
+      </c>
+      <c r="B65" s="5">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>42</v>
+      </c>
+      <c r="B66" s="5">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>43</v>
+      </c>
+      <c r="B67" s="5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>44</v>
+      </c>
+      <c r="B68" s="5">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>45</v>
+      </c>
+      <c r="B69" s="5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>46</v>
+      </c>
+      <c r="B70" s="5">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>47</v>
+      </c>
+      <c r="B71" s="5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>48</v>
+      </c>
+      <c r="B72" s="5">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>49</v>
+      </c>
+      <c r="B73" s="5">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>50</v>
+      </c>
+      <c r="B74" s="5">
+        <v>144</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2003,7 +2301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1682CA-3BD7-CA42-8A85-53F8AFB35EE2}">
   <dimension ref="A1:O102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated PID Code for 0610
</commit_message>
<xml_diff>
--- a/SensorCalibration.xlsx
+++ b/SensorCalibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yewheng/Desktop/CZ3004-MDP-Arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8814784C-7A11-2645-A642-027F418F061C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE932FD1-C501-DD4E-BCD6-8C911E7448F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16860" yWindow="480" windowWidth="11940" windowHeight="16220" activeTab="1" xr2:uid="{2238A5C0-9490-7B40-8416-1163AD9190C2}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="11940" windowHeight="16220" activeTab="1" xr2:uid="{2238A5C0-9490-7B40-8416-1163AD9190C2}"/>
   </bookViews>
   <sheets>
     <sheet name="01 Oct (2cm Interval)" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="15">
   <si>
     <t>SRSensorFront1</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>SRSensorFront1 (Old)</t>
   </si>
 </sst>
 </file>
@@ -125,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -138,9 +141,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1347,16 +1347,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272BC585-879A-D54C-8DC8-951D497B05AE}">
-  <dimension ref="A1:O74"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:B74"/>
+    <sheetView tabSelected="1" topLeftCell="B70" zoomScale="89" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E85" sqref="D55:E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="7" width="20.83203125" customWidth="1"/>
-    <col min="10" max="15" width="20.83203125" customWidth="1"/>
+    <col min="10" max="15" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" x14ac:dyDescent="0.25">
@@ -1379,7 +1379,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>1</v>
@@ -1419,444 +1419,638 @@
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1">
+        <v>3182.24</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="M2" s="1">
+        <v>6852.53</v>
+      </c>
+      <c r="N2" s="1">
+        <v>8273.8700000000008</v>
+      </c>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>625</v>
+      </c>
+      <c r="C3" s="5">
+        <v>652</v>
+      </c>
+      <c r="D3" s="5">
+        <v>604</v>
+      </c>
+      <c r="E3" s="5">
+        <v>662</v>
+      </c>
+      <c r="F3" s="5">
+        <v>658</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1">
+        <v>5.5339999999999998</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="M3" s="1">
+        <v>9.9003099999999993</v>
+      </c>
+      <c r="N3" s="1">
+        <v>11.013500000000001</v>
+      </c>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>565</v>
+      </c>
+      <c r="C4" s="5">
+        <v>644</v>
+      </c>
+      <c r="D4" s="5">
+        <v>543</v>
+      </c>
+      <c r="E4" s="5">
+        <v>622</v>
+      </c>
+      <c r="F4" s="5">
+        <v>650</v>
+      </c>
       <c r="G4" s="6"/>
       <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1">
+        <v>-71.561000000000007</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="M4" s="1">
+        <v>16.189299999999999</v>
+      </c>
+      <c r="N4" s="1">
+        <v>61.616100000000003</v>
+      </c>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>531</v>
+      </c>
+      <c r="C5" s="5">
+        <v>617</v>
+      </c>
+      <c r="D5" s="5">
+        <v>506</v>
+      </c>
+      <c r="E5" s="5">
+        <v>570</v>
+      </c>
+      <c r="F5" s="5">
+        <v>592</v>
+      </c>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>480</v>
+      </c>
+      <c r="C6" s="5">
+        <v>560</v>
+      </c>
+      <c r="D6" s="5">
+        <v>458</v>
+      </c>
+      <c r="E6" s="5">
+        <v>519</v>
+      </c>
+      <c r="F6" s="5">
+        <v>534</v>
+      </c>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>445</v>
+      </c>
+      <c r="C7" s="5">
+        <v>517</v>
+      </c>
+      <c r="D7" s="5">
+        <v>426</v>
+      </c>
+      <c r="E7" s="5">
+        <v>480</v>
+      </c>
+      <c r="F7" s="5">
+        <v>487</v>
+      </c>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="B8" s="5">
+        <v>413</v>
+      </c>
+      <c r="C8" s="5">
+        <v>473</v>
+      </c>
+      <c r="D8" s="5">
+        <v>396</v>
+      </c>
+      <c r="E8" s="5">
+        <v>447</v>
+      </c>
+      <c r="F8" s="5">
+        <v>454</v>
+      </c>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="B9" s="5">
+        <v>392</v>
+      </c>
+      <c r="C9" s="5">
+        <v>447</v>
+      </c>
+      <c r="D9" s="5">
+        <v>377</v>
+      </c>
+      <c r="E9" s="5">
+        <v>415</v>
+      </c>
+      <c r="F9" s="5">
+        <v>419</v>
+      </c>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>365</v>
+      </c>
+      <c r="C10" s="5">
+        <v>417</v>
+      </c>
+      <c r="D10" s="5">
+        <v>354</v>
+      </c>
+      <c r="E10" s="5">
+        <v>388</v>
+      </c>
+      <c r="F10" s="5">
+        <v>394</v>
+      </c>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="5">
-        <v>455.6</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+        <v>341</v>
+      </c>
+      <c r="C11" s="5">
+        <v>390</v>
+      </c>
+      <c r="D11" s="5">
+        <v>335</v>
+      </c>
+      <c r="E11" s="5">
+        <v>356</v>
+      </c>
+      <c r="F11" s="5">
+        <v>360</v>
+      </c>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5">
-        <v>422</v>
+        <v>326</v>
       </c>
       <c r="C12" s="5">
-        <v>517</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+        <v>365</v>
+      </c>
+      <c r="D12" s="5">
+        <v>322</v>
+      </c>
+      <c r="E12" s="5">
+        <v>337</v>
+      </c>
+      <c r="F12" s="5">
+        <v>340</v>
+      </c>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="5">
-        <v>394.8</v>
+        <v>310</v>
       </c>
       <c r="C13" s="5">
-        <v>477</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+        <v>350</v>
+      </c>
+      <c r="D13" s="5">
+        <v>303</v>
+      </c>
+      <c r="E13" s="5">
+        <v>325</v>
+      </c>
+      <c r="F13" s="5">
+        <v>325</v>
+      </c>
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="5">
-        <v>364.9</v>
+        <v>301</v>
       </c>
       <c r="C14" s="5">
-        <v>446</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+        <v>332</v>
+      </c>
+      <c r="D14" s="5">
+        <v>289</v>
+      </c>
+      <c r="E14" s="5">
+        <v>307</v>
+      </c>
+      <c r="F14" s="5">
+        <v>308</v>
+      </c>
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5">
-        <v>351.1</v>
+        <v>286</v>
       </c>
       <c r="C15" s="5">
-        <v>413</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+        <v>310</v>
+      </c>
+      <c r="D15" s="5">
+        <v>271</v>
+      </c>
+      <c r="E15" s="5">
+        <v>295</v>
+      </c>
+      <c r="F15" s="5">
+        <v>292</v>
+      </c>
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="5">
-        <v>328.9</v>
+        <v>273</v>
       </c>
       <c r="C16" s="5">
-        <v>389</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+        <v>297</v>
+      </c>
+      <c r="D16" s="5">
+        <v>259</v>
+      </c>
+      <c r="E16" s="5">
+        <v>284</v>
+      </c>
+      <c r="F16" s="5">
+        <v>279</v>
+      </c>
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5">
-        <v>317.5</v>
+        <v>263</v>
       </c>
       <c r="C17" s="5">
-        <v>367</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+        <v>285</v>
+      </c>
+      <c r="D17" s="5">
+        <v>256</v>
+      </c>
+      <c r="E17" s="5">
+        <v>270</v>
+      </c>
+      <c r="F17" s="5">
+        <v>266</v>
+      </c>
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="5">
-        <v>300.8</v>
+        <v>250</v>
       </c>
       <c r="C18" s="5">
-        <v>348</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+        <v>275</v>
+      </c>
+      <c r="D18" s="5">
+        <v>249</v>
+      </c>
+      <c r="E18" s="5">
+        <v>260</v>
+      </c>
+      <c r="F18" s="5">
+        <v>258</v>
+      </c>
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="5">
-        <v>284.5</v>
+        <v>243</v>
       </c>
       <c r="C19" s="5">
-        <v>329</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+        <v>265</v>
+      </c>
+      <c r="D19" s="5">
+        <v>235</v>
+      </c>
+      <c r="E19" s="5">
+        <v>251</v>
+      </c>
+      <c r="F19" s="5">
+        <v>243</v>
+      </c>
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="5">
-        <v>277</v>
+        <v>235</v>
       </c>
       <c r="C20" s="5">
-        <v>314</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+        <v>255</v>
+      </c>
+      <c r="D20" s="5">
+        <v>227</v>
+      </c>
+      <c r="E20" s="5">
+        <v>242</v>
+      </c>
+      <c r="F20" s="5">
+        <v>233</v>
+      </c>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5">
-        <v>265</v>
+        <v>225</v>
       </c>
       <c r="C21" s="5">
-        <v>300</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+        <v>238</v>
+      </c>
+      <c r="D21" s="5">
+        <v>217</v>
+      </c>
+      <c r="E21" s="5">
+        <v>230</v>
+      </c>
+      <c r="F21" s="5">
+        <v>225</v>
+      </c>
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5">
-        <v>256.7</v>
+        <v>222</v>
       </c>
       <c r="C22" s="5">
-        <v>288</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+        <v>239</v>
+      </c>
+      <c r="D22" s="5">
+        <v>211</v>
+      </c>
+      <c r="E22" s="5">
+        <v>222</v>
+      </c>
+      <c r="F22" s="5">
+        <v>216</v>
+      </c>
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="5">
-        <v>251.2</v>
+        <v>216</v>
       </c>
       <c r="C23" s="5">
-        <v>274</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+        <v>222</v>
+      </c>
+      <c r="D23" s="5">
+        <v>205</v>
+      </c>
+      <c r="E23" s="5">
+        <v>218</v>
+      </c>
+      <c r="F23" s="5">
+        <v>211</v>
+      </c>
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="5">
-        <v>245.3</v>
+        <v>200</v>
       </c>
       <c r="C24" s="5">
-        <v>259</v>
-      </c>
-      <c r="D24" s="5"/>
+        <v>197</v>
+      </c>
+      <c r="D24" s="5">
+        <v>198</v>
+      </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="5">
-        <v>235</v>
+        <v>196</v>
       </c>
       <c r="C25" s="5">
-        <v>248</v>
-      </c>
-      <c r="D25" s="5"/>
+        <v>193</v>
+      </c>
+      <c r="D25" s="5">
+        <v>190</v>
+      </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="5">
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="C26" s="5">
-        <v>243</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>185</v>
+      </c>
+      <c r="D26" s="5">
+        <v>183</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="5">
-        <v>221</v>
+        <v>188</v>
       </c>
       <c r="C27" s="5">
-        <v>236</v>
-      </c>
-      <c r="D27" s="5"/>
+        <v>181</v>
+      </c>
+      <c r="D27" s="5">
+        <v>178</v>
+      </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="5">
-        <v>222.9</v>
+        <v>183</v>
       </c>
       <c r="C28" s="5">
-        <v>226</v>
-      </c>
-      <c r="D28" s="5"/>
+        <v>172</v>
+      </c>
+      <c r="D28" s="5">
+        <v>171</v>
+      </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="5">
-        <v>213.6</v>
+        <v>177</v>
       </c>
       <c r="C29" s="5">
-        <v>218</v>
-      </c>
-      <c r="D29" s="5"/>
+        <v>167</v>
+      </c>
+      <c r="D29" s="5">
+        <v>163</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="5">
-        <v>208.8</v>
+        <v>177</v>
       </c>
       <c r="C30" s="5">
-        <v>213</v>
-      </c>
-      <c r="D30" s="5"/>
+        <v>163</v>
+      </c>
+      <c r="D30" s="5">
+        <v>159</v>
+      </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="5">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="C31" s="5">
-        <v>207</v>
-      </c>
-      <c r="D31" s="5"/>
+        <v>159</v>
+      </c>
+      <c r="D31" s="5">
+        <v>155</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="5">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="C32" s="5">
-        <v>204</v>
+        <v>155</v>
       </c>
       <c r="D32" s="5">
-        <v>203</v>
+        <v>151</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -1864,14 +2058,16 @@
     </row>
     <row r="33" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="5">
-        <v>191.6</v>
-      </c>
-      <c r="C33" s="5"/>
+        <v>175</v>
+      </c>
+      <c r="C33" s="5">
+        <v>150</v>
+      </c>
       <c r="D33" s="5">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -1879,417 +2075,937 @@
     </row>
     <row r="34" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="5">
-        <v>187</v>
-      </c>
+      <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="5">
-        <v>183</v>
-      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="5">
-        <v>180</v>
-      </c>
+      <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="5">
-        <v>174</v>
-      </c>
+      <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="5">
-        <v>171</v>
-      </c>
+      <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="5">
-        <v>161</v>
-      </c>
+      <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="5">
-        <v>166</v>
-      </c>
+      <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="5">
-        <v>157</v>
-      </c>
+      <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="5">
-        <v>158</v>
-      </c>
+      <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="5">
-        <v>152</v>
-      </c>
+      <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="5">
-        <v>147</v>
-      </c>
+      <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="5">
-        <v>142</v>
-      </c>
+      <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
     <row r="46" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
-      <c r="D46" s="5">
-        <v>138</v>
-      </c>
+      <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
     </row>
     <row r="47" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
-      <c r="D47" s="5">
-        <v>132</v>
-      </c>
+      <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
-      <c r="D48" s="5">
-        <v>131</v>
-      </c>
+      <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
     </row>
     <row r="49" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
-      <c r="D49" s="5">
-        <v>128</v>
-      </c>
+      <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
     </row>
     <row r="50" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
-      <c r="D50" s="5">
-        <v>124</v>
-      </c>
+      <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
     </row>
     <row r="51" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
-      <c r="D51" s="5">
-        <v>137</v>
-      </c>
+      <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
-      <c r="D52" s="5">
-        <v>144</v>
-      </c>
+      <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
     </row>
+    <row r="53" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>50</v>
+      </c>
+    </row>
     <row r="54" spans="1:7" ht="20" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>30</v>
-      </c>
-      <c r="B54" s="5">
-        <v>203</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B55" s="5">
-        <v>193</v>
+        <v>625</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0</v>
+      </c>
+      <c r="D55" s="5">
+        <v>652</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="5">
+        <v>604</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B56" s="5">
-        <v>187</v>
+        <v>565</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="5">
+        <v>644</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56" s="5">
+        <v>543</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="B57" s="5">
-        <v>183</v>
+        <v>531</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2</v>
+      </c>
+      <c r="D57" s="5">
+        <v>617</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2</v>
+      </c>
+      <c r="F57" s="5">
+        <v>506</v>
+      </c>
+      <c r="G57" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B58" s="5">
-        <v>180</v>
+        <v>480</v>
+      </c>
+      <c r="C58" s="1">
+        <v>3</v>
+      </c>
+      <c r="D58" s="5">
+        <v>560</v>
+      </c>
+      <c r="E58" s="1">
+        <v>3</v>
+      </c>
+      <c r="F58" s="5">
+        <v>458</v>
+      </c>
+      <c r="G58" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="B59" s="5">
-        <v>174</v>
+        <v>445</v>
+      </c>
+      <c r="C59" s="1">
+        <v>4</v>
+      </c>
+      <c r="D59" s="5">
+        <v>517</v>
+      </c>
+      <c r="E59" s="1">
+        <v>4</v>
+      </c>
+      <c r="F59" s="5">
+        <v>426</v>
+      </c>
+      <c r="G59" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="B60" s="5">
-        <v>171</v>
+        <v>413</v>
+      </c>
+      <c r="C60" s="1">
+        <v>5</v>
+      </c>
+      <c r="D60" s="5">
+        <v>473</v>
+      </c>
+      <c r="E60" s="1">
+        <v>5</v>
+      </c>
+      <c r="F60" s="5">
+        <v>396</v>
+      </c>
+      <c r="G60" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="B61" s="5">
-        <v>161</v>
+        <v>392</v>
+      </c>
+      <c r="C61" s="1">
+        <v>6</v>
+      </c>
+      <c r="D61" s="5">
+        <v>447</v>
+      </c>
+      <c r="E61" s="1">
+        <v>6</v>
+      </c>
+      <c r="F61" s="5">
+        <v>377</v>
+      </c>
+      <c r="G61" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="B62" s="5">
-        <v>166</v>
+        <v>365</v>
+      </c>
+      <c r="C62" s="1">
+        <v>7</v>
+      </c>
+      <c r="D62" s="5">
+        <v>417</v>
+      </c>
+      <c r="E62" s="1">
+        <v>7</v>
+      </c>
+      <c r="F62" s="5">
+        <v>354</v>
+      </c>
+      <c r="G62" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B63" s="5">
-        <v>157</v>
+        <v>341</v>
+      </c>
+      <c r="C63" s="1">
+        <v>8</v>
+      </c>
+      <c r="D63" s="5">
+        <v>390</v>
+      </c>
+      <c r="E63" s="1">
+        <v>8</v>
+      </c>
+      <c r="F63" s="5">
+        <v>335</v>
+      </c>
+      <c r="G63" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B64" s="5">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+      <c r="C64" s="1">
+        <v>9</v>
+      </c>
+      <c r="D64" s="5">
+        <v>365</v>
+      </c>
+      <c r="E64" s="1">
+        <v>9</v>
+      </c>
+      <c r="F64" s="5">
+        <v>322</v>
+      </c>
+      <c r="G64" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="B65" s="5">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+      <c r="C65" s="1">
+        <v>10</v>
+      </c>
+      <c r="D65" s="5">
+        <v>350</v>
+      </c>
+      <c r="E65" s="1">
+        <v>10</v>
+      </c>
+      <c r="F65" s="5">
+        <v>303</v>
+      </c>
+      <c r="G65" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="B66" s="5">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+      <c r="C66" s="1">
+        <v>11</v>
+      </c>
+      <c r="D66" s="5">
+        <v>332</v>
+      </c>
+      <c r="E66" s="1">
+        <v>11</v>
+      </c>
+      <c r="F66" s="5">
+        <v>289</v>
+      </c>
+      <c r="G66" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B67" s="5">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="C67" s="1">
+        <v>12</v>
+      </c>
+      <c r="D67" s="5">
+        <v>310</v>
+      </c>
+      <c r="E67" s="1">
+        <v>12</v>
+      </c>
+      <c r="F67" s="5">
+        <v>271</v>
+      </c>
+      <c r="G67" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="B68" s="5">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+      <c r="C68" s="1">
+        <v>13</v>
+      </c>
+      <c r="D68" s="5">
+        <v>297</v>
+      </c>
+      <c r="E68" s="1">
+        <v>13</v>
+      </c>
+      <c r="F68" s="5">
+        <v>259</v>
+      </c>
+      <c r="G68" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B69" s="5">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+      <c r="C69" s="1">
+        <v>14</v>
+      </c>
+      <c r="D69" s="5">
+        <v>285</v>
+      </c>
+      <c r="E69" s="1">
+        <v>14</v>
+      </c>
+      <c r="F69" s="5">
+        <v>256</v>
+      </c>
+      <c r="G69" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="B70" s="5">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="C70" s="1">
+        <v>15</v>
+      </c>
+      <c r="D70" s="5">
+        <v>275</v>
+      </c>
+      <c r="E70" s="1">
+        <v>15</v>
+      </c>
+      <c r="F70" s="5">
+        <v>249</v>
+      </c>
+      <c r="G70" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="B71" s="5">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="C71" s="1">
+        <v>16</v>
+      </c>
+      <c r="D71" s="5">
+        <v>265</v>
+      </c>
+      <c r="E71" s="1">
+        <v>16</v>
+      </c>
+      <c r="F71" s="5">
+        <v>235</v>
+      </c>
+      <c r="G71" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B72" s="5">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="C72" s="1">
+        <v>17</v>
+      </c>
+      <c r="D72" s="5">
+        <v>255</v>
+      </c>
+      <c r="E72" s="1">
+        <v>17</v>
+      </c>
+      <c r="F72" s="5">
+        <v>227</v>
+      </c>
+      <c r="G72" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B73" s="5">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="C73" s="1">
+        <v>18</v>
+      </c>
+      <c r="D73" s="5">
+        <v>238</v>
+      </c>
+      <c r="E73" s="1">
+        <v>18</v>
+      </c>
+      <c r="F73" s="5">
+        <v>217</v>
+      </c>
+      <c r="G73" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="B74" s="5">
-        <v>144</v>
+        <v>222</v>
+      </c>
+      <c r="C74" s="1">
+        <v>19</v>
+      </c>
+      <c r="D74" s="5">
+        <v>239</v>
+      </c>
+      <c r="E74" s="1">
+        <v>19</v>
+      </c>
+      <c r="F74" s="5">
+        <v>211</v>
+      </c>
+      <c r="G74" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>20</v>
+      </c>
+      <c r="B75" s="5">
+        <v>216</v>
+      </c>
+      <c r="C75" s="1">
+        <v>20</v>
+      </c>
+      <c r="D75" s="5">
+        <v>222</v>
+      </c>
+      <c r="E75" s="1">
+        <v>20</v>
+      </c>
+      <c r="F75" s="5">
+        <v>205</v>
+      </c>
+      <c r="G75" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>21</v>
+      </c>
+      <c r="B76" s="5">
+        <v>200</v>
+      </c>
+      <c r="C76" s="1">
+        <v>21</v>
+      </c>
+      <c r="D76" s="5">
+        <v>197</v>
+      </c>
+      <c r="E76" s="1">
+        <v>21</v>
+      </c>
+      <c r="F76" s="5">
+        <v>198</v>
+      </c>
+      <c r="G76" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>22</v>
+      </c>
+      <c r="B77" s="5">
+        <v>196</v>
+      </c>
+      <c r="C77" s="1">
+        <v>22</v>
+      </c>
+      <c r="D77" s="5">
+        <v>193</v>
+      </c>
+      <c r="E77" s="1">
+        <v>22</v>
+      </c>
+      <c r="F77" s="5">
+        <v>190</v>
+      </c>
+      <c r="G77" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>23</v>
+      </c>
+      <c r="B78" s="5">
+        <v>193</v>
+      </c>
+      <c r="C78" s="1">
+        <v>23</v>
+      </c>
+      <c r="D78" s="5">
+        <v>185</v>
+      </c>
+      <c r="E78" s="1">
+        <v>23</v>
+      </c>
+      <c r="F78" s="5">
+        <v>183</v>
+      </c>
+      <c r="G78" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>24</v>
+      </c>
+      <c r="B79" s="5">
+        <v>188</v>
+      </c>
+      <c r="C79" s="1">
+        <v>24</v>
+      </c>
+      <c r="D79" s="5">
+        <v>181</v>
+      </c>
+      <c r="E79" s="1">
+        <v>24</v>
+      </c>
+      <c r="F79" s="5">
+        <v>178</v>
+      </c>
+      <c r="G79" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>25</v>
+      </c>
+      <c r="B80" s="5">
+        <v>183</v>
+      </c>
+      <c r="C80" s="1">
+        <v>25</v>
+      </c>
+      <c r="D80" s="5">
+        <v>172</v>
+      </c>
+      <c r="E80" s="1">
+        <v>25</v>
+      </c>
+      <c r="F80" s="5">
+        <v>171</v>
+      </c>
+      <c r="G80" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>26</v>
+      </c>
+      <c r="B81" s="5">
+        <v>177</v>
+      </c>
+      <c r="C81" s="1">
+        <v>26</v>
+      </c>
+      <c r="D81" s="5">
+        <v>167</v>
+      </c>
+      <c r="E81" s="1">
+        <v>26</v>
+      </c>
+      <c r="F81" s="5">
+        <v>163</v>
+      </c>
+      <c r="G81" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>27</v>
+      </c>
+      <c r="B82" s="5">
+        <v>177</v>
+      </c>
+      <c r="C82" s="1">
+        <v>27</v>
+      </c>
+      <c r="D82" s="5">
+        <v>163</v>
+      </c>
+      <c r="E82" s="1">
+        <v>27</v>
+      </c>
+      <c r="F82" s="5">
+        <v>159</v>
+      </c>
+      <c r="G82" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>28</v>
+      </c>
+      <c r="B83" s="5">
+        <v>176</v>
+      </c>
+      <c r="C83" s="1">
+        <v>28</v>
+      </c>
+      <c r="D83" s="5">
+        <v>159</v>
+      </c>
+      <c r="E83" s="1">
+        <v>28</v>
+      </c>
+      <c r="F83" s="5">
+        <v>155</v>
+      </c>
+      <c r="G83" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>29</v>
+      </c>
+      <c r="B84" s="5">
+        <v>176</v>
+      </c>
+      <c r="C84" s="1">
+        <v>29</v>
+      </c>
+      <c r="D84" s="5">
+        <v>155</v>
+      </c>
+      <c r="E84" s="1">
+        <v>29</v>
+      </c>
+      <c r="F84" s="5">
+        <v>151</v>
+      </c>
+      <c r="G84" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>30</v>
+      </c>
+      <c r="B85" s="5">
+        <v>175</v>
+      </c>
+      <c r="C85" s="1">
+        <v>30</v>
+      </c>
+      <c r="D85" s="5">
+        <v>150</v>
+      </c>
+      <c r="E85" s="1">
+        <v>30</v>
+      </c>
+      <c r="F85" s="5">
+        <v>150</v>
+      </c>
+      <c r="G85" s="1">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2387,7 +3103,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="7"/>
+      <c r="G3" s="6"/>
       <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
@@ -2407,7 +3123,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="7"/>
+      <c r="G4" s="6"/>
       <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2427,7 +3143,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="7"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -2438,7 +3154,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="7"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -2449,7 +3165,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="7"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -2460,7 +3176,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="7"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -2471,7 +3187,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="7"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -2482,7 +3198,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -2493,7 +3209,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -2504,7 +3220,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -2515,7 +3231,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -2526,7 +3242,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -2537,7 +3253,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -2548,7 +3264,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -2559,7 +3275,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -2570,7 +3286,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="7"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -2581,7 +3297,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="7"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -2592,7 +3308,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="7"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -2603,7 +3319,7 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="7"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -2614,7 +3330,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="7"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">

</xml_diff>